<commit_message>
clasification outcome csv added
</commit_message>
<xml_diff>
--- a/results/manual_perceptron_wyniki_classification_our_train_test.xlsx
+++ b/results/manual_perceptron_wyniki_classification_our_train_test.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
       <c r="D2" t="n">
         <v>9</v>
@@ -536,34 +536,34 @@
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3160381262065581</v>
+        <v>0.3339766362425737</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8572156731909847</v>
+        <v>0.8491251482799527</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8570018430534548</v>
+        <v>0.8488367430909034</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8575200086421324</v>
+        <v>0.8491450062394154</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8571781417462455</v>
+        <v>0.8489083586281878</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3187274835625197</v>
+        <v>0.3394845138433463</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8534089645200756</v>
+        <v>0.8499610721832944</v>
       </c>
       <c r="N2" t="n">
-        <v>0.853802093111615</v>
+        <v>0.8500480337349755</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8534108182678263</v>
+        <v>0.849961948626192</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8536064108517269</v>
+        <v>0.8500049890009947</v>
       </c>
     </row>
     <row r="3">
@@ -574,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05</v>
+        <v>0.005</v>
       </c>
       <c r="D3" t="n">
         <v>9</v>
@@ -583,37 +583,37 @@
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3153997976057301</v>
+        <v>0.3181139860465447</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8582670192434426</v>
+        <v>0.8559645610913406</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8581914376235619</v>
+        <v>0.8556319718881987</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8581323833996197</v>
+        <v>0.8561335245688194</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8580837008385533</v>
+        <v>0.8558002786095092</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3175101076983191</v>
+        <v>0.3201224312687553</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8545211878545211</v>
+        <v>0.8548548548548549</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8546117758065468</v>
+        <v>0.8550335356163692</v>
       </c>
       <c r="O3" t="n">
-        <v>0.854522076724237</v>
+        <v>0.8548561024705188</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8545669239115898</v>
+        <v>0.8549448098374343</v>
       </c>
     </row>
     <row r="4">
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0.01</v>
@@ -633,37 +633,37 @@
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3134520671813198</v>
+        <v>0.3169250466192468</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8583329214445763</v>
+        <v>0.8562199321207328</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8579827624404101</v>
+        <v>0.8558298050588314</v>
       </c>
       <c r="J4" t="n">
-        <v>0.858363756164899</v>
+        <v>0.856249984659181</v>
       </c>
       <c r="K4" t="n">
-        <v>0.858091537072579</v>
+        <v>0.8559627929396519</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3169035329443492</v>
+        <v>0.3204532971964326</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8542987431876321</v>
+        <v>0.8527416305194083</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8545945945945946</v>
+        <v>0.852870329533254</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8543003495382374</v>
+        <v>0.8527426925528168</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8544474467342112</v>
+        <v>0.8528065062672748</v>
       </c>
     </row>
     <row r="5">
@@ -671,10 +671,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="D5" t="n">
         <v>9</v>
@@ -686,45 +686,45 @@
         <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3076576805106348</v>
+        <v>0.3120146045247023</v>
       </c>
       <c r="H5" t="n">
-        <v>0.860690984578885</v>
+        <v>0.8585604899828655</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8606588104181251</v>
+        <v>0.8583137030723754</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8608212055857283</v>
+        <v>0.8588359340477654</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8606577923413153</v>
+        <v>0.8584938306705879</v>
       </c>
       <c r="L5" t="n">
-        <v>0.3102689685899899</v>
+        <v>0.3144930130058981</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8599710821933044</v>
+        <v>0.8550772995217439</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8602400879763683</v>
+        <v>0.855216059172877</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8599726020212256</v>
+        <v>0.8550783986952684</v>
       </c>
       <c r="P5" t="n">
-        <v>0.8601063242023174</v>
+        <v>0.855147223393972</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
       <c r="D6" t="n">
         <v>9</v>
@@ -736,45 +736,45 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3155352171316833</v>
+        <v>0.329496037607915</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8588107124027943</v>
+        <v>0.850543075326216</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8586224419099195</v>
+        <v>0.8503908357648842</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8586370941070594</v>
+        <v>0.8506238637019027</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8585496662346273</v>
+        <v>0.8504221901515276</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3203815915247505</v>
+        <v>0.3346029867588532</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8558558558558559</v>
+        <v>0.8515181848515182</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8560762818877652</v>
+        <v>0.8515289288096544</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8558572395583863</v>
+        <v>0.8515184922749279</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8559667467098149</v>
+        <v>0.8515237105103128</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05</v>
+        <v>0.005</v>
       </c>
       <c r="D7" t="n">
         <v>9</v>
@@ -783,42 +783,42 @@
         <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>0.311756328381661</v>
+        <v>0.3162134482425001</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8589898840121259</v>
+        <v>0.8563537959667854</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8592594684420066</v>
+        <v>0.8560682847447464</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8590006704349399</v>
+        <v>0.8562996138430253</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8590378272274245</v>
+        <v>0.8561040639130008</v>
       </c>
       <c r="L7" t="n">
-        <v>0.3152164517475291</v>
+        <v>0.3207164410056326</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8555221888555222</v>
+        <v>0.8525191858525192</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8556739173437466</v>
+        <v>0.8526600734301545</v>
       </c>
       <c r="O7" t="n">
-        <v>0.8555233375161805</v>
+        <v>0.8525202973648063</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8555986208046944</v>
+        <v>0.8525901796686587</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
         <v>16</v>
@@ -833,48 +833,48 @@
         <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3111731641455078</v>
+        <v>0.3136899351427446</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8606631820877818</v>
+        <v>0.858077550415184</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8605161710607087</v>
+        <v>0.8579331692447818</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8605601358420494</v>
+        <v>0.8580533424932385</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8604557142302968</v>
+        <v>0.8579081425177856</v>
       </c>
       <c r="L8" t="n">
-        <v>0.3127194535306158</v>
+        <v>0.3172799447655308</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8557446335224113</v>
+        <v>0.8539650761872984</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8559237591970462</v>
+        <v>0.8543030829894973</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8557458811490822</v>
+        <v>0.8539667938674447</v>
       </c>
       <c r="P8" t="n">
-        <v>0.8558348109304513</v>
+        <v>0.8541349053276199</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="D9" t="n">
         <v>9</v>
@@ -883,37 +883,2837 @@
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3046400294397741</v>
+        <v>0.311345879120532</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8633095673520496</v>
+        <v>0.860273947212337</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8636961553890969</v>
+        <v>0.8601095455889365</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8633228084894399</v>
+        <v>0.8604309732660443</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8634160001736353</v>
+        <v>0.8601897191239426</v>
       </c>
       <c r="L9" t="n">
-        <v>0.3041695677124474</v>
+        <v>0.3127721932705662</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8619730841953064</v>
+        <v>0.8560783005227449</v>
       </c>
       <c r="N9" t="n">
-        <v>0.8620438359358938</v>
+        <v>0.8562611681303702</v>
       </c>
       <c r="O9" t="n">
-        <v>0.8619738618235366</v>
+        <v>0.8560795605239511</v>
       </c>
       <c r="P9" t="n">
-        <v>0.862008847459667</v>
+        <v>0.8561703546966817</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="n">
+        <v>32</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.3279256182815894</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.8518775948991697</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.8516058963032624</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.8517570408179556</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.8515995113219703</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.3322358146812676</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.8512957401846291</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.851321983856127</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.8512962207909935</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.8513091021286441</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="n">
+        <v>32</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.3148855653012576</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.857071512126005</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.8569303207787929</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.8571727838617001</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.8569705421565779</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.3185735193976722</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.853075297519742</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.8532602135926041</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.8530765698542073</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.8531683818411178</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
+        <v>32</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.3122522138391328</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.8587499588111243</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.8583871475514079</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.8588782624498427</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.8585550185226292</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.3155217951275019</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.8545211878545211</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.8548357597265965</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.8545228436895087</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.8546792730667698</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>32</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.308823110529594</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.8609463556082773</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.8608943710626435</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.8609580253019058</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.8608450551011833</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.3122983733967744</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.8558558558558559</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.8561174885086515</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.8558573632624624</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.8559874061232504</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="n">
+        <v>64</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.3262101525155858</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.8526838671411626</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.8525307335362984</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.8525827341727598</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.8524709084858515</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.3305736424304452</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.85229674118563</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.8523122771684403</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.8522971104707089</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.8523046937521019</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="n">
+        <v>64</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D15" t="n">
+        <v>9</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3139200919763696</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.857488549492553</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.8571185537984334</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.8574883565375025</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.8572245214875767</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.3175918372098212</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.854076298520743</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.8543452528212461</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.8540778306461509</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.8542115208036899</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>64</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.3106295862703578</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.8598898609463556</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.8596141385406048</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.8597568568055663</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.8596058889545175</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.3146674630309396</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.8546324101879658</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.8550428647916226</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.8546343010620737</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.8548385341093508</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="n">
+        <v>64</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.3067283780350706</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8618916403057862</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.8617362945959365</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.8617495213910589</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.8616625500539626</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.3107250629036569</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.8587476365254143</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.8591574110071608</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.8587495150800217</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.8589534146186489</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="n">
+        <v>8</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D18" t="n">
+        <v>9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.3322609091571101</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.8507932977461448</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.8506445294050684</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.8507754220719249</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.8506250310187909</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.3367414630487008</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.8509620731842954</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.8510673687755506</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.8509630362324291</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.8510151993062561</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" t="n">
+        <v>8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.3177735517347559</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.8565206109134046</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.8563889167058774</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.8567237462155907</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.8564711322803253</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.3216463260944175</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.8535201868535202</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.8537843990699652</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.8535217066016412</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.853653032626383</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="n">
+        <v>8</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D20" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.3139376928766926</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.8583051189534731</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.8579735704947915</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.8583187866890222</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.8580624514604713</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.3156283069692455</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.8557446335224113</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.8559851461293126</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.855746079075604</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.8558655959079401</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>8</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D21" t="n">
+        <v>9</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.3152077703097833</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.8574936981020167</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.857314195991547</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.8575577273172228</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.8573540000185148</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.3153427936508502</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.8551885218551886</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.8554007346442857</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.8551898808086487</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.8552952947311486</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>16</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D22" t="n">
+        <v>9</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.3264242342102718</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.8512937425860024</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.8512022977409441</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.8512546112816168</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.8511417149020971</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.3317859657409669</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.8502947391836281</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.8503610707017977</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.8502955042969847</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.8503282862354814</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" t="n">
+        <v>16</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D23" t="n">
+        <v>9</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.314573461244353</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.8589950326215896</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.8586594388293796</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.8589377529444124</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.8587153485305777</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.3189225723506903</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.8536314091869648</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.8540247840583896</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.853633262937467</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.8538289786151755</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" t="n">
+        <v>16</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D24" t="n">
+        <v>9</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.3120891423777127</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.8591340450771057</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.8588887643326725</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.8590784776711605</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.8588989066801116</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.3133057970806019</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.8566344121899677</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.8568673343430837</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.8566358330133521</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.8567515680398267</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" t="n">
+        <v>16</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D25" t="n">
+        <v>9</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.3060703271479014</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.8625589000922631</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.8627024285706333</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.8626044936398782</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.8625689866520878</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.3076392124150923</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.8597486375264153</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.8599226488080238</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.8597498604618021</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.8598362459542449</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" t="n">
+        <v>32</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D26" t="n">
+        <v>9</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.3223500451217335</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.854935868920522</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.8546083588469194</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.8551634380674141</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.8548036364590139</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.3270175689557827</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.8534089645200756</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.8534716207776114</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.8534097049311413</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.8534406617314009</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2</v>
+      </c>
+      <c r="B27" t="n">
+        <v>32</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D27" t="n">
+        <v>9</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.3125997844137492</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.8593564650059312</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.8589209244037279</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.8593823654885107</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.859072580519797</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.3156936566739375</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.8538538538538538</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.8541772983820642</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.8538555344214014</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.8540163860943393</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" t="n">
+        <v>32</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D28" t="n">
+        <v>9</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.3078788148138936</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.8618308867141163</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8616428157802448</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.861830131531072</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.8616568705214475</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.3109935440974981</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.8577466355244133</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.8580139883534706</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.8577481553248172</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.8578810512456138</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2</v>
+      </c>
+      <c r="B29" t="n">
+        <v>32</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D29" t="n">
+        <v>9</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.3053844228006216</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.8622757265717675</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.8624822520650662</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.862180801283907</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.8622475672787736</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.3087654005687651</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.8603047491936381</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.8605122278661355</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.8603060834695728</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.860409143320382</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" t="n">
+        <v>64</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D30" t="n">
+        <v>9</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.3194685245681825</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.8556257825886384</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.8554907492326558</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.8557668382402978</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.8555492086598642</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.3242280112896206</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.8546324101879658</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.8547062264666405</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.8546332124662041</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.8546697179070349</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2</v>
+      </c>
+      <c r="B31" t="n">
+        <v>64</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D31" t="n">
+        <v>9</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.3102683962572919</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.861029763081587</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.8607021167717841</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.8609063341966942</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.8607251049968402</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.314055022881025</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.8560783005227449</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.856394246784</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.8560799563769946</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.8562370727396367</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" t="n">
+        <v>64</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D32" t="n">
+        <v>9</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.3063768332226002</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.8612521830104125</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.8613270962450221</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.861165716045539</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.8611631451004713</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.3112875664193483</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.8585251918585252</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.8588338542928498</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.8585268230022287</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.8586803112018737</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2</v>
+      </c>
+      <c r="B33" t="n">
+        <v>64</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D33" t="n">
+        <v>9</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.300125414103921</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.8646945432977462</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.8649356065360443</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.864553568645309</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.8646568981545747</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.3056888000457416</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.8605271938605272</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.8607504953189291</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.860528577620844</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.8606395221644014</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" t="n">
+        <v>8</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D34" t="n">
+        <v>9</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.3293490296897034</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.8494865806642943</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.8492258053293357</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.8496131630308188</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.8493354330604023</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.3337070726284291</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.8509620731842954</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.8510162601626017</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.8509627640834616</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.8509895112822955</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" t="n">
+        <v>8</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D35" t="n">
+        <v>9</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.318010159790512</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.8556082773164624</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.855342302799965</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.855485264417021</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.8553315856562971</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.3222093207841845</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.8505171838505172</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.8508567582265729</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.8505189138584193</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.8506878024993995</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" t="n">
+        <v>8</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D36" t="n">
+        <v>9</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.3149295505334415</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.8588107124027943</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.8587539602801334</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.8589024945738636</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.8587429682213017</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.316409047929526</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.8558558558558559</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.8559980664811691</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.855856967409419</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.8559275111302724</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3</v>
+      </c>
+      <c r="B37" t="n">
+        <v>8</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D37" t="n">
+        <v>9</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.3133006891778872</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.8591391936865691</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.8595201265972474</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.8592528546819754</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.8592912846436577</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.3149849378990418</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.8560783005227449</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.8561963795455281</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.8560793131157989</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.8561378423288111</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" t="n">
+        <v>16</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D38" t="n">
+        <v>9</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.3240653426756895</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.8526282621589562</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.8522755893004546</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.8526510191561872</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.8523816764209369</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.3290944271368267</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.8521855188521855</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.8522939107449365</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.8521864942858612</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.852240199130703</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>3</v>
+      </c>
+      <c r="B39" t="n">
+        <v>16</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D39" t="n">
+        <v>9</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.3122856085019234</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.859806453473046</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.8595898231107459</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.8596353569358764</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.8595330318220987</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.3149934882932913</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.8551885218551886</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.8554760389405101</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0.8551901034759856</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.8553330473113904</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>3</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D40" t="n">
+        <v>9</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.3109301986430686</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.860412959667853</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.8605474183914663</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.8606269767030988</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.8605015208915904</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.3135905458639325</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.8549660771882994</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.8551556111627974</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.8549673619165621</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.8550614761785013</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>3</v>
+      </c>
+      <c r="B41" t="n">
+        <v>16</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D41" t="n">
+        <v>9</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.3063793137374697</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.8619142941874259</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.862460167208461</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.8620549361001648</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.8621701413977698</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.3068281316687958</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.8584139695250806</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.858414384324204</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.8584140296256417</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.8584142069748861</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" t="n">
+        <v>32</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D42" t="n">
+        <v>9</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" t="n">
+        <v>3</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.3182978396694218</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.8568212897060761</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.8563909172877797</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.85683049243549</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.8565319478737188</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.3209125312308432</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.8544099655210766</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.8545547743638662</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.854411089427161</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.8544829258552054</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" t="n">
+        <v>32</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D43" t="n">
+        <v>9</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.3101818841285872</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.8600515272835113</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.8601196189596816</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.8601848010831969</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.8600686003673047</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.313387920966868</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.857079301523746</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.8572383281874441</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.8570804749444816</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.8571593942984563</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>3</v>
+      </c>
+      <c r="B44" t="n">
+        <v>32</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D44" t="n">
+        <v>9</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.3050288313392537</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.8624528387373138</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.8626738643571542</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.8624274463509395</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.8624634828456912</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.3091716671510576</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.8578578578578578</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.8579597571152386</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.85785879625048</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.8579092737125288</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>3</v>
+      </c>
+      <c r="B45" t="n">
+        <v>32</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D45" t="n">
+        <v>9</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2991020836598819</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.8651167292737577</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.8655215637309169</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.8650494999539683</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.8651945659695657</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.3053276114337714</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.8607496385274163</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.8607541188998322</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.8607498347313544</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.8607519768102624</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>3</v>
+      </c>
+      <c r="B46" t="n">
+        <v>64</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D46" t="n">
+        <v>9</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.3169931681375716</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.8575596003031501</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.8573186964758027</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.8577134557941385</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.857432148583129</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.3214971818670579</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.8539650761872984</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.8542043928811858</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.8539665217184773</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.8540854407374695</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>3</v>
+      </c>
+      <c r="B47" t="n">
+        <v>64</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D47" t="n">
+        <v>9</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.3074342077130251</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.8613633929748253</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.8613820677060576</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.8612189815341517</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.8612157396391369</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.3136039288281542</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.8557446335224113</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.8561042049482461</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.8557464007062019</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0.8559252654338103</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3</v>
+      </c>
+      <c r="B48" t="n">
+        <v>64</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D48" t="n">
+        <v>9</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.3020151312270314</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.8634485798075656</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.8635421589260976</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.8632807743462196</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.8633307938918718</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.308738111799916</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.8567456345234123</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.8569510768511124</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.8567469687553193</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0.8568490106481822</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3</v>
+      </c>
+      <c r="B49" t="n">
+        <v>64</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D49" t="n">
+        <v>9</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.296153477223647</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.8664841999472782</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.867312469761365</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.8664338337185673</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.8667773039963076</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.3052272812675988</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.8556334111889667</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.8556737072371599</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.8556340031826585</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.8556538547493222</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>4</v>
+      </c>
+      <c r="B50" t="n">
+        <v>8</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D50" t="n">
+        <v>9</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.6926148911055976</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.6594637620271516</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.7397163868295374</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.661572740636575</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.6958546094461927</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.6925968325152643</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.6704482260037815</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.7488212917706218</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.6704794324654915</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0.7074882245193853</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>4</v>
+      </c>
+      <c r="B51" t="n">
+        <v>8</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D51" t="n">
+        <v>9</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.3154764436372599</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.8578777843679979</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.8575469901631497</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.8579745050185326</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.8576779186184974</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.3190800039626322</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.8538538538538538</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.8539546234325984</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0.8538547921969448</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0.8539047048969179</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>4</v>
+      </c>
+      <c r="B52" t="n">
+        <v>8</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D52" t="n">
+        <v>9</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.3166539578547099</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.8583782292078554</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.8584482516720648</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.8584166688665341</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.858344127211088</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.3179358251281005</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.8535201868535202</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.8535849748538296</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.8535209396363694</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0.8535529560440877</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" t="n">
+        <v>8</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D53" t="n">
+        <v>9</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.3132312924686819</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.8598342559641492</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.8604758090022067</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.859930132363691</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.8601139269520571</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.3165309237520972</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.8541875208541875</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.8541953563595097</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.8541872592718679</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0.8541913077965002</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>4</v>
+      </c>
+      <c r="B54" t="n">
+        <v>16</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D54" t="n">
+        <v>9</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>3</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.3290844917160695</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.8504092114801635</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.8503132327652203</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.8503941992483353</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.8502705253650247</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.3324490719832223</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.8499610721832944</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.8501896624202023</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.8499624929241268</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0.8500760624952937</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>4</v>
+      </c>
+      <c r="B55" t="n">
+        <v>16</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D55" t="n">
+        <v>9</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" t="n">
+        <v>3</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.3128850566016068</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.8582721678529064</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.8582240721247416</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.8584526716724946</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.8582502925726443</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.3147851418717533</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.8569680791903014</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.8571171549260468</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0.8569692154984383</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0.8570431788280618</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>4</v>
+      </c>
+      <c r="B56" t="n">
+        <v>16</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D56" t="n">
+        <v>9</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" t="n">
+        <v>3</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.3030120273217119</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.8634485798075656</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.8640207309224786</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.8633964471602699</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.8636161039190831</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.3058411591374644</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.8589700811923034</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.8589772924078757</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.8589698320395536</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0.8589735622075159</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>4</v>
+      </c>
+      <c r="B57" t="n">
+        <v>16</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D57" t="n">
+        <v>9</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.3022488336751091</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.8639160735468565</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.8647093538097641</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.863918207474233</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.8642146410699911</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.3052418428364775</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.8579690801913025</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.8580397315818356</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0.8579682990986426</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0.8580040138534746</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>4</v>
+      </c>
+      <c r="B58" t="n">
+        <v>32</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D58" t="n">
+        <v>9</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.3178267945907797</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.8569376482799527</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.8565684522264299</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.8569503515841694</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.856682098910229</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.3222641717932864</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.8537426315204093</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.8540156937548838</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.8537441760120972</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0.853879913299108</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>4</v>
+      </c>
+      <c r="B59" t="n">
+        <v>32</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D59" t="n">
+        <v>9</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.3092050022774392</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.8612799855015157</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.8613236022033971</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.8612392400648853</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.8611988496320477</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.3136439260177742</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.8577466355244133</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.8579722079625827</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0.8577480316207411</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0.8578601051461995</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>4</v>
+      </c>
+      <c r="B60" t="n">
+        <v>32</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D60" t="n">
+        <v>9</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F60" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.3033898736235681</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.8634207773164624</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.8638497228671753</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.8633314427002095</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.8635051723051929</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.3063777288090645</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.8598598598598599</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.8598702454163805</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0.8598595612364865</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0.8598649032932446</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>4</v>
+      </c>
+      <c r="B61" t="n">
+        <v>32</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D61" t="n">
+        <v>9</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.3005321302438331</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.8644824205878476</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.8650118844295412</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.8645174178492158</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.864677159403372</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.3037616542281065</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.8600823045267489</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0.8600849338950003</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0.8600821543510188</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0.8600835441207639</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>4</v>
+      </c>
+      <c r="B62" t="n">
+        <v>64</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D62" t="n">
+        <v>9</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.3154995287434354</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.8581887603795968</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.8579267016046583</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.8583017234311348</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.8580305257795969</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.3201226557705009</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.8534089645200756</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.8536688085096142</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0.8534104718964132</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0.853539620655648</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>4</v>
+      </c>
+      <c r="B63" t="n">
+        <v>64</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D63" t="n">
+        <v>9</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.3036032223507377</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.8639490246474232</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.8641615427590221</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.8637049873564288</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.8638496587886636</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0.3099508226990075</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.8583027471916361</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.858354162276612</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0.8583034134407943</v>
+      </c>
+      <c r="P63" t="n">
+        <v>0.8583287871085697</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>4</v>
+      </c>
+      <c r="B64" t="n">
+        <v>64</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D64" t="n">
+        <v>9</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.3009579888608814</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.8648665068538289</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.8656278971491658</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.864944518636347</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.8651904784870614</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.3072818703129324</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.8579690801913025</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.857985935683786</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0.857969461916958</v>
+      </c>
+      <c r="P64" t="n">
+        <v>0.8579776987212951</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>4</v>
+      </c>
+      <c r="B65" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D65" t="n">
+        <v>9</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2</v>
+      </c>
+      <c r="F65" t="n">
+        <v>3</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.295372935983996</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.8675581998813761</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.8683274291334969</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.8676581460579026</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.8678996390724565</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.3068467465531399</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.8575241908575242</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.8575460480021536</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0.857523756130774</v>
+      </c>
+      <c r="P65" t="n">
+        <v>0.857534901921593</v>
       </c>
     </row>
   </sheetData>
@@ -955,7 +3755,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-11-13 09:47:32</t>
+          <t>2025-11-13 11:19:53</t>
         </is>
       </c>
     </row>

</xml_diff>